<commit_message>
fixed a test, and fixed the file output code
</commit_message>
<xml_diff>
--- a/src/testData/NameTest.xlsx
+++ b/src/testData/NameTest.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t xml:space="preserve">NameSeq</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">Yea's Jewellers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gloucester</t>
   </si>
   <si>
     <t xml:space="preserve">Tommy</t>
@@ -326,7 +329,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -437,7 +440,7 @@
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>19</v>
@@ -461,18 +464,18 @@
         <v>32519</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>19</v>

</xml_diff>